<commit_message>
code done but untested
</commit_message>
<xml_diff>
--- a/Reference/pinout.xlsx
+++ b/Reference/pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewd\Documents\GitHub\buttonBox\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9E6DB-CC76-482B-8E63-9A04443A3E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9231815-E73D-4811-BAD2-30D2964238DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{52D6E8A3-AEE4-4EFF-A70E-B0B3F144ADFE}"/>
+    <workbookView xWindow="4710" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{52D6E8A3-AEE4-4EFF-A70E-B0B3F144ADFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>T1</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>EN3_CLK</t>
+  </si>
+  <si>
+    <t>EN3_DAT</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +727,9 @@
       <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="1">
         <v>28</v>
       </c>
@@ -733,7 +741,9 @@
       <c r="B16" s="1">
         <v>14</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E16" s="1">
         <v>29</v>
       </c>

</xml_diff>